<commit_message>
User Creationg Project: - Improved search functionality of users and user group by using deep search api of checkpoint instead of basic text search - Improved code by directly accessing dicts and lists without dumping to json - Removed json dependencies
</commit_message>
<xml_diff>
--- a/Checkpoint_User_Mobility/config/User-Mobility-Data.xlsx
+++ b/Checkpoint_User_Mobility/config/User-Mobility-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_User_Mobility\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD51E9A8-1ABA-4532-B8D4-7D40A5599E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F947F40-0795-478B-A0DA-6809E7899F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="3324" windowWidth="15132" windowHeight="7980" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,9 +509,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{65149EB1-CE65-4FC2-9B50-80B87A676724}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{3EBD452D-0665-48B7-89DD-131AE2C9F1E5}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{8DEA0D80-1AE7-4E0E-BC2F-492C29B4572F}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{AFE061DD-B172-4F67-8BF2-22C3F8659459}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{8DEA0D80-1AE7-4E0E-BC2F-492C29B4572F}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{3EBD452D-0665-48B7-89DD-131AE2C9F1E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>